<commit_message>
updated 2 icdc scripts to resolve wait time issue
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Canine_StudyUBC-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC02_Canine_StudyUBC-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\inputfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\updated code\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D73CF1-9EC6-4366-8825-10EA86728409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCE8123-82E9-4EC9-A80A-8A2B2A1492BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -77,6 +77,41 @@
 	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
   <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
+ WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN coalesce(f.file_name, '') AS `File Name`, 
+        coalesce(f.file_type, '') AS `File Type`, 
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `File Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
 WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
@@ -93,43 +128,7 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
- WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
   </si>
 </sst>
 </file>
@@ -501,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,12 +529,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -552,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -569,7 +568,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Timing issue fix - keywords, updated tc1,2 in ubc01
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Canine_StudyUBC-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC02_Canine_StudyUBC-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\inputfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\updated code\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D73CF1-9EC6-4366-8825-10EA86728409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCE8123-82E9-4EC9-A80A-8A2B2A1492BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -77,6 +77,41 @@
 	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
   <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
+ WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN coalesce(f.file_name, '') AS `File Name`, 
+        coalesce(f.file_type, '') AS `File Type`, 
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `File Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
 WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
@@ -93,43 +128,7 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
- WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['UBC01'] and demo.breed in ['Border Collie','Chihuahua','Maltese','Scottish Terrier']and diag.disease_term in ['Bladder Cancer'] and diag.primary_disease_site in ['Bladder, Urethra', 'Bladder, Urethra, Prostate']
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
   </si>
 </sst>
 </file>
@@ -501,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,12 +529,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -552,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -569,7 +568,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>

</xml_diff>